<commit_message>
generating pdfs from the excel content
</commit_message>
<xml_diff>
--- a/docs/Gerenciamento de Qualidade/CheckList_ehSoja.xlsx
+++ b/docs/Gerenciamento de Qualidade/CheckList_ehSoja.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25601"/>
-  <workbookPr defaultThemeVersion="124226"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25629"/>
+  <workbookPr hidePivotFieldList="1" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\api-6-semestre\docs\Gerenciamento de Qualidade\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B537A29-46BC-4989-98FC-2A8D782BB376}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B240516A-2BC4-46EF-A45A-88445E8A99A8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -347,29 +347,17 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" pivotButton="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" indent="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -386,17 +374,171 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" pivotButton="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="44">
+    <dxf>
+      <alignment wrapText="1"/>
+    </dxf>
+    <dxf>
+      <alignment wrapText="1"/>
+    </dxf>
+    <dxf>
+      <alignment wrapText="1"/>
+    </dxf>
+    <dxf>
+      <alignment wrapText="1"/>
+    </dxf>
+    <dxf>
+      <alignment wrapText="1"/>
+    </dxf>
+    <dxf>
+      <alignment wrapText="1"/>
+    </dxf>
+    <dxf>
+      <alignment wrapText="1"/>
+    </dxf>
+    <dxf>
+      <alignment wrapText="1"/>
+    </dxf>
+    <dxf>
+      <alignment wrapText="1"/>
+    </dxf>
+    <dxf>
+      <alignment wrapText="1"/>
+    </dxf>
+    <dxf>
+      <alignment wrapText="1"/>
+    </dxf>
+    <dxf>
+      <alignment wrapText="1"/>
+    </dxf>
+    <dxf>
+      <alignment wrapText="1"/>
+    </dxf>
+    <dxf>
+      <alignment wrapText="0"/>
+    </dxf>
+    <dxf>
+      <alignment wrapText="0"/>
+    </dxf>
+    <dxf>
+      <alignment wrapText="0"/>
+    </dxf>
+    <dxf>
+      <alignment wrapText="0"/>
+    </dxf>
+    <dxf>
+      <alignment wrapText="0"/>
+    </dxf>
+    <dxf>
+      <alignment wrapText="0"/>
+    </dxf>
+    <dxf>
+      <alignment wrapText="0"/>
+    </dxf>
+    <dxf>
+      <alignment wrapText="0"/>
+    </dxf>
+    <dxf>
+      <alignment wrapText="0"/>
+    </dxf>
+    <dxf>
+      <alignment wrapText="0"/>
+    </dxf>
+    <dxf>
+      <alignment wrapText="0"/>
+    </dxf>
+    <dxf>
+      <alignment wrapText="0"/>
+    </dxf>
+    <dxf>
+      <alignment wrapText="0"/>
+    </dxf>
+    <dxf>
+      <alignment wrapText="0"/>
+    </dxf>
+    <dxf>
+      <alignment wrapText="1"/>
+    </dxf>
+    <dxf>
+      <alignment wrapText="1" indent="0"/>
+    </dxf>
+    <dxf>
+      <alignment wrapText="1" indent="0"/>
+    </dxf>
+    <dxf>
+      <alignment wrapText="1" indent="0"/>
+    </dxf>
+    <dxf>
+      <alignment wrapText="1" indent="0"/>
+    </dxf>
+    <dxf>
+      <alignment wrapText="1" indent="0"/>
+    </dxf>
+    <dxf>
+      <alignment wrapText="1" indent="0"/>
+    </dxf>
+    <dxf>
+      <alignment wrapText="1" indent="0"/>
+    </dxf>
+    <dxf>
+      <alignment wrapText="1" indent="0"/>
+    </dxf>
+    <dxf>
+      <alignment wrapText="1" indent="0"/>
+    </dxf>
+    <dxf>
+      <alignment wrapText="1" indent="0"/>
+    </dxf>
+    <dxf>
+      <alignment wrapText="1" indent="0"/>
+    </dxf>
+    <dxf>
+      <alignment wrapText="1" indent="0"/>
+    </dxf>
+    <dxf>
+      <alignment wrapText="1" indent="0"/>
+    </dxf>
+    <dxf>
+      <alignment wrapText="1"/>
+    </dxf>
+    <dxf>
+      <alignment wrapText="1"/>
+    </dxf>
+    <dxf>
+      <alignment wrapText="1" indent="0"/>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -585,7 +727,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{00000000-0007-0000-0100-000000000000}" name="PivotTable1" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="4" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="4" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{00000000-0007-0000-0100-000000000000}" name="PivotTable1" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="4" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="A3:A36" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="3">
     <pivotField axis="axisRow" showAll="0">
@@ -606,7 +748,6 @@
     <pivotField axis="axisRow" showAll="0">
       <items count="23">
         <item n="[x] Conjunto de habilidades requeridas por função identificado." x="11"/>
-        <item n="[x] Cronograma e Orçamento criado e validado pela equipe de projeto com todas as atividades do projeto e os recursos necessários para executá-las" x="15"/>
         <item n="[x] Definido abordagem, ferramentas e workflow usado para avaliar os pedidos de mudança." x="20"/>
         <item n="[x] Definido objetivos do projeto" x="3"/>
         <item n="[x] Definido processo que assegurará o cumprimento dos requisitos do cliente e as políticas e padrões da empresa." x="8"/>
@@ -627,6 +768,7 @@
         <item n="[x] Processo de auditoria para avaliar o desempenho do projeto definido." x="7"/>
         <item n="[x] Projeto aderente com as políticas e padrões definidos pela empresa." x="6"/>
         <item n="[x] Riscos potenciais identificados." x="17"/>
+        <item n="[x] Cronograma e Orçamento criado e validado pela equipe de projeto com todas as atividades do projeto e os recursos necessários para executá-las" x="15"/>
         <item t="default"/>
       </items>
     </pivotField>
@@ -646,97 +788,97 @@
       <x/>
     </i>
     <i r="1">
-      <x v="5"/>
+      <x v="4"/>
     </i>
     <i>
       <x v="1"/>
     </i>
     <i r="1">
-      <x v="21"/>
+      <x v="20"/>
     </i>
     <i>
       <x v="2"/>
     </i>
     <i r="1">
-      <x v="12"/>
+      <x v="11"/>
     </i>
     <i>
       <x v="3"/>
     </i>
     <i r="1">
+      <x v="1"/>
+    </i>
+    <i r="1">
+      <x v="7"/>
+    </i>
+    <i>
+      <x v="4"/>
+    </i>
+    <i r="1">
+      <x v="12"/>
+    </i>
+    <i r="1">
+      <x v="16"/>
+    </i>
+    <i r="1">
+      <x v="17"/>
+    </i>
+    <i>
+      <x v="5"/>
+    </i>
+    <i r="1">
       <x v="2"/>
+    </i>
+    <i r="1">
+      <x v="5"/>
+    </i>
+    <i r="1">
+      <x v="6"/>
+    </i>
+    <i>
+      <x v="6"/>
+    </i>
+    <i r="1">
+      <x v="21"/>
+    </i>
+    <i>
+      <x v="7"/>
+    </i>
+    <i r="1">
+      <x v="3"/>
     </i>
     <i r="1">
       <x v="8"/>
     </i>
+    <i r="1">
+      <x v="9"/>
+    </i>
+    <i r="1">
+      <x v="18"/>
+    </i>
+    <i r="1">
+      <x v="19"/>
+    </i>
     <i>
-      <x v="4"/>
+      <x v="8"/>
+    </i>
+    <i r="1">
+      <x/>
     </i>
     <i r="1">
       <x v="13"/>
     </i>
     <i r="1">
-      <x v="17"/>
+      <x v="14"/>
     </i>
     <i r="1">
-      <x v="18"/>
+      <x v="15"/>
     </i>
     <i>
-      <x v="5"/>
-    </i>
-    <i r="1">
-      <x v="3"/>
-    </i>
-    <i r="1">
-      <x v="6"/>
-    </i>
-    <i r="1">
-      <x v="7"/>
-    </i>
-    <i>
-      <x v="6"/>
-    </i>
-    <i r="1">
-      <x v="1"/>
-    </i>
-    <i>
-      <x v="7"/>
-    </i>
-    <i r="1">
-      <x v="4"/>
-    </i>
-    <i r="1">
       <x v="9"/>
     </i>
     <i r="1">
       <x v="10"/>
-    </i>
-    <i r="1">
-      <x v="19"/>
-    </i>
-    <i r="1">
-      <x v="20"/>
-    </i>
-    <i>
-      <x v="8"/>
-    </i>
-    <i r="1">
-      <x/>
-    </i>
-    <i r="1">
-      <x v="14"/>
-    </i>
-    <i r="1">
-      <x v="15"/>
-    </i>
-    <i r="1">
-      <x v="16"/>
-    </i>
-    <i>
-      <x v="9"/>
-    </i>
-    <i r="1">
-      <x v="11"/>
     </i>
     <i t="grand">
       <x/>
@@ -745,6 +887,304 @@
   <colItems count="1">
     <i/>
   </colItems>
+  <formats count="28">
+    <format dxfId="43">
+      <pivotArea type="all" dataOnly="0" outline="0" fieldPosition="0"/>
+    </format>
+    <format dxfId="40">
+      <pivotArea field="0" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisRow" fieldPosition="0"/>
+    </format>
+    <format dxfId="39">
+      <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
+        <references count="1">
+          <reference field="0" count="0"/>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="38">
+      <pivotArea dataOnly="0" labelOnly="1" grandRow="1" outline="0" fieldPosition="0"/>
+    </format>
+    <format dxfId="37">
+      <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
+        <references count="2">
+          <reference field="0" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="1" count="1">
+            <x v="4"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="36">
+      <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
+        <references count="2">
+          <reference field="0" count="1" selected="0">
+            <x v="1"/>
+          </reference>
+          <reference field="1" count="1">
+            <x v="20"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="35">
+      <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
+        <references count="2">
+          <reference field="0" count="1" selected="0">
+            <x v="2"/>
+          </reference>
+          <reference field="1" count="1">
+            <x v="11"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="34">
+      <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
+        <references count="2">
+          <reference field="0" count="1" selected="0">
+            <x v="3"/>
+          </reference>
+          <reference field="1" count="2">
+            <x v="1"/>
+            <x v="7"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="33">
+      <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
+        <references count="2">
+          <reference field="0" count="1" selected="0">
+            <x v="4"/>
+          </reference>
+          <reference field="1" count="3">
+            <x v="12"/>
+            <x v="16"/>
+            <x v="17"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="32">
+      <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
+        <references count="2">
+          <reference field="0" count="1" selected="0">
+            <x v="5"/>
+          </reference>
+          <reference field="1" count="3">
+            <x v="2"/>
+            <x v="5"/>
+            <x v="6"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="31">
+      <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
+        <references count="2">
+          <reference field="0" count="1" selected="0">
+            <x v="6"/>
+          </reference>
+          <reference field="1" count="1">
+            <x v="21"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="30">
+      <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
+        <references count="2">
+          <reference field="0" count="1" selected="0">
+            <x v="7"/>
+          </reference>
+          <reference field="1" count="5">
+            <x v="3"/>
+            <x v="8"/>
+            <x v="9"/>
+            <x v="18"/>
+            <x v="19"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="29">
+      <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
+        <references count="2">
+          <reference field="0" count="1" selected="0">
+            <x v="8"/>
+          </reference>
+          <reference field="1" count="4">
+            <x v="0"/>
+            <x v="13"/>
+            <x v="14"/>
+            <x v="15"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="28">
+      <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
+        <references count="2">
+          <reference field="0" count="1" selected="0">
+            <x v="9"/>
+          </reference>
+          <reference field="1" count="1">
+            <x v="10"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="27">
+      <pivotArea type="all" dataOnly="0" outline="0" fieldPosition="0"/>
+    </format>
+    <format dxfId="12">
+      <pivotArea field="0" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisRow" fieldPosition="0"/>
+    </format>
+    <format dxfId="11">
+      <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
+        <references count="1">
+          <reference field="0" count="0"/>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="10">
+      <pivotArea dataOnly="0" labelOnly="1" grandRow="1" outline="0" fieldPosition="0"/>
+    </format>
+    <format dxfId="9">
+      <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
+        <references count="2">
+          <reference field="0" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="1" count="1">
+            <x v="4"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="8">
+      <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
+        <references count="2">
+          <reference field="0" count="1" selected="0">
+            <x v="1"/>
+          </reference>
+          <reference field="1" count="1">
+            <x v="20"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="7">
+      <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
+        <references count="2">
+          <reference field="0" count="1" selected="0">
+            <x v="2"/>
+          </reference>
+          <reference field="1" count="1">
+            <x v="11"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="6">
+      <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
+        <references count="2">
+          <reference field="0" count="1" selected="0">
+            <x v="3"/>
+          </reference>
+          <reference field="1" count="2">
+            <x v="1"/>
+            <x v="7"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="5">
+      <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
+        <references count="2">
+          <reference field="0" count="1" selected="0">
+            <x v="4"/>
+          </reference>
+          <reference field="1" count="3">
+            <x v="12"/>
+            <x v="16"/>
+            <x v="17"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="4">
+      <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
+        <references count="2">
+          <reference field="0" count="1" selected="0">
+            <x v="5"/>
+          </reference>
+          <reference field="1" count="3">
+            <x v="2"/>
+            <x v="5"/>
+            <x v="6"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="3">
+      <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
+        <references count="2">
+          <reference field="0" count="1" selected="0">
+            <x v="6"/>
+          </reference>
+          <reference field="1" count="1">
+            <x v="21"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="2">
+      <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
+        <references count="2">
+          <reference field="0" count="1" selected="0">
+            <x v="7"/>
+          </reference>
+          <reference field="1" count="5">
+            <x v="3"/>
+            <x v="8"/>
+            <x v="9"/>
+            <x v="18"/>
+            <x v="19"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="1">
+      <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
+        <references count="2">
+          <reference field="0" count="1" selected="0">
+            <x v="8"/>
+          </reference>
+          <reference field="1" count="4">
+            <x v="0"/>
+            <x v="13"/>
+            <x v="14"/>
+            <x v="15"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="0">
+      <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
+        <references count="2">
+          <reference field="0" count="1" selected="0">
+            <x v="9"/>
+          </reference>
+          <reference field="1" count="1">
+            <x v="10"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+  </formats>
   <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
@@ -1080,340 +1520,341 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E24"/>
   <sheetViews>
-    <sheetView topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="E24" sqref="E24"/>
+    <sheetView topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="E2" sqref="E1:E1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="49.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="49.5703125" style="8"/>
-    <col min="2" max="2" width="48.140625" style="8" customWidth="1"/>
-    <col min="3" max="3" width="6.28515625" style="11" customWidth="1"/>
-    <col min="4" max="4" width="6.140625" style="11" customWidth="1"/>
-    <col min="5" max="16384" width="49.5703125" style="8"/>
+    <col min="1" max="1" width="22.42578125" style="3" customWidth="1"/>
+    <col min="2" max="2" width="48.140625" style="3" customWidth="1"/>
+    <col min="3" max="3" width="6.28515625" style="5" customWidth="1"/>
+    <col min="4" max="4" width="6.140625" style="5" customWidth="1"/>
+    <col min="5" max="5" width="29" style="12" customWidth="1"/>
+    <col min="6" max="16384" width="49.5703125" style="3"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" s="16" t="s">
+      <c r="A1" s="13" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="16"/>
-      <c r="C1" s="16"/>
-      <c r="D1" s="16"/>
-      <c r="E1" s="17"/>
+      <c r="B1" s="13"/>
+      <c r="C1" s="13"/>
+      <c r="D1" s="13"/>
+      <c r="E1" s="14"/>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" s="12" t="s">
+      <c r="A2" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="12" t="s">
+      <c r="B2" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="12" t="s">
+      <c r="C2" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="D2" s="12" t="s">
+      <c r="D2" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="E2" s="12" t="s">
+      <c r="E2" s="6" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A3" s="4" t="s">
+    <row r="3" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B3" s="4" t="s">
+      <c r="B3" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C3" s="13" t="s">
+      <c r="C3" s="7" t="s">
         <v>44</v>
       </c>
-      <c r="D3" s="13"/>
-      <c r="E3" s="5"/>
-    </row>
-    <row r="4" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A4" s="6" t="s">
+      <c r="D3" s="7"/>
+      <c r="E3" s="10"/>
+    </row>
+    <row r="4" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="6" t="s">
+      <c r="B4" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="C4" s="14" t="s">
+      <c r="C4" s="8" t="s">
         <v>44</v>
       </c>
-      <c r="D4" s="14"/>
-      <c r="E4" s="7"/>
-    </row>
-    <row r="5" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A5" s="4" t="s">
+      <c r="D4" s="8"/>
+      <c r="E4" s="11"/>
+    </row>
+    <row r="5" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B5" s="4" t="s">
+      <c r="B5" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C5" s="13" t="s">
+      <c r="C5" s="7" t="s">
         <v>44</v>
       </c>
-      <c r="D5" s="13"/>
-      <c r="E5" s="5"/>
+      <c r="D5" s="7"/>
+      <c r="E5" s="10"/>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" s="9" t="s">
+      <c r="A6" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="B6" s="9" t="s">
+      <c r="B6" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="C6" s="15" t="s">
+      <c r="C6" s="9" t="s">
         <v>44</v>
       </c>
-      <c r="D6" s="15"/>
+      <c r="D6" s="9"/>
     </row>
     <row r="7" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A7" s="9" t="s">
+      <c r="A7" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="B7" s="9" t="s">
+      <c r="B7" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="C7" s="15" t="s">
+      <c r="C7" s="9" t="s">
         <v>44</v>
       </c>
-      <c r="D7" s="15"/>
+      <c r="D7" s="9"/>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8" s="9" t="s">
+      <c r="A8" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="B8" s="9" t="s">
+      <c r="B8" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="C8" s="15" t="s">
+      <c r="C8" s="9" t="s">
         <v>44</v>
       </c>
-      <c r="D8" s="15"/>
+      <c r="D8" s="9"/>
     </row>
     <row r="9" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A9" s="6" t="s">
+      <c r="A9" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="B9" s="6" t="s">
+      <c r="B9" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="C9" s="14" t="s">
+      <c r="C9" s="8" t="s">
         <v>44</v>
       </c>
-      <c r="D9" s="14"/>
-      <c r="E9" s="7"/>
+      <c r="D9" s="8"/>
+      <c r="E9" s="11"/>
     </row>
     <row r="10" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A10" s="6" t="s">
+      <c r="A10" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="B10" s="6" t="s">
+      <c r="B10" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="C10" s="14"/>
-      <c r="D10" s="14" t="s">
+      <c r="C10" s="8"/>
+      <c r="D10" s="8" t="s">
         <v>44</v>
       </c>
-      <c r="E10" s="7" t="s">
+      <c r="E10" s="11" t="s">
         <v>45</v>
       </c>
     </row>
     <row r="11" spans="1:5" ht="45" x14ac:dyDescent="0.25">
-      <c r="A11" s="6" t="s">
+      <c r="A11" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="B11" s="6" t="s">
+      <c r="B11" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="C11" s="14" t="s">
+      <c r="C11" s="8" t="s">
         <v>44</v>
       </c>
-      <c r="D11" s="14"/>
-      <c r="E11" s="7"/>
+      <c r="D11" s="8"/>
+      <c r="E11" s="11"/>
     </row>
     <row r="12" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A12" s="6" t="s">
+      <c r="A12" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="B12" s="6" t="s">
+      <c r="B12" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="C12" s="14" t="s">
+      <c r="C12" s="8" t="s">
         <v>44</v>
       </c>
-      <c r="D12" s="14"/>
-      <c r="E12" s="7"/>
+      <c r="D12" s="8"/>
+      <c r="E12" s="11"/>
     </row>
     <row r="13" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A13" s="6" t="s">
+      <c r="A13" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="B13" s="6" t="s">
+      <c r="B13" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="C13" s="14" t="s">
+      <c r="C13" s="8" t="s">
         <v>44</v>
       </c>
-      <c r="D13" s="14"/>
-      <c r="E13" s="7"/>
-    </row>
-    <row r="14" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A14" s="9" t="s">
+      <c r="D13" s="8"/>
+      <c r="E13" s="11"/>
+    </row>
+    <row r="14" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A14" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="B14" s="9" t="s">
+      <c r="B14" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="C14" s="15"/>
-      <c r="D14" s="15" t="s">
+      <c r="C14" s="9"/>
+      <c r="D14" s="9" t="s">
         <v>44</v>
       </c>
-      <c r="E14" s="8" t="s">
+      <c r="E14" s="12" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="15" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A15" s="9" t="s">
+    <row r="15" spans="1:5" ht="75" x14ac:dyDescent="0.25">
+      <c r="A15" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="B15" s="9" t="s">
+      <c r="B15" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="C15" s="15"/>
-      <c r="D15" s="15" t="s">
+      <c r="C15" s="9"/>
+      <c r="D15" s="9" t="s">
         <v>44</v>
       </c>
-      <c r="E15" s="8" t="s">
+      <c r="E15" s="12" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="16" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A16" s="9" t="s">
+    <row r="16" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A16" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="B16" s="9" t="s">
+      <c r="B16" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="C16" s="15" t="s">
+      <c r="C16" s="9" t="s">
         <v>44</v>
       </c>
-      <c r="D16" s="15"/>
-    </row>
-    <row r="17" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A17" s="9" t="s">
+      <c r="D16" s="9"/>
+    </row>
+    <row r="17" spans="1:5" ht="75" x14ac:dyDescent="0.25">
+      <c r="A17" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="B17" s="9" t="s">
+      <c r="B17" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="C17" s="15"/>
-      <c r="D17" s="15" t="s">
+      <c r="C17" s="9"/>
+      <c r="D17" s="9" t="s">
         <v>44</v>
       </c>
-      <c r="E17" s="8" t="s">
+      <c r="E17" s="12" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="18" spans="1:5" ht="45" x14ac:dyDescent="0.25">
-      <c r="A18" s="6" t="s">
+    <row r="18" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+      <c r="A18" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="B18" s="6" t="s">
+      <c r="B18" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="C18" s="14" t="s">
+      <c r="C18" s="8" t="s">
         <v>44</v>
       </c>
-      <c r="D18" s="14"/>
-      <c r="E18" s="7"/>
+      <c r="D18" s="8"/>
+      <c r="E18" s="11"/>
     </row>
     <row r="19" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A19" s="9" t="s">
+      <c r="A19" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="B19" s="9" t="s">
+      <c r="B19" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="C19" s="15" t="s">
+      <c r="C19" s="9" t="s">
         <v>44</v>
       </c>
-      <c r="D19" s="15"/>
+      <c r="D19" s="9"/>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A20" s="6" t="s">
+      <c r="A20" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="B20" s="6" t="s">
+      <c r="B20" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="C20" s="14" t="s">
+      <c r="C20" s="8" t="s">
         <v>44</v>
       </c>
-      <c r="D20" s="14"/>
-      <c r="E20" s="7"/>
+      <c r="D20" s="8"/>
+      <c r="E20" s="11"/>
     </row>
     <row r="21" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A21" s="9" t="s">
+      <c r="A21" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="B21" s="9" t="s">
+      <c r="B21" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="C21" s="15" t="s">
+      <c r="C21" s="9" t="s">
         <v>44</v>
       </c>
-      <c r="D21" s="15"/>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A22" s="6" t="s">
+      <c r="D21" s="9"/>
+    </row>
+    <row r="22" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A22" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="B22" s="6" t="s">
+      <c r="B22" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="C22" s="14" t="s">
+      <c r="C22" s="8" t="s">
         <v>44</v>
       </c>
-      <c r="D22" s="14"/>
-      <c r="E22" s="7"/>
-    </row>
-    <row r="23" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A23" s="6" t="s">
+      <c r="D22" s="8"/>
+      <c r="E22" s="11"/>
+    </row>
+    <row r="23" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+      <c r="A23" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="B23" s="6" t="s">
+      <c r="B23" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="C23" s="14"/>
-      <c r="D23" s="14" t="s">
+      <c r="C23" s="8"/>
+      <c r="D23" s="8" t="s">
         <v>44</v>
       </c>
-      <c r="E23" s="7" t="s">
+      <c r="E23" s="11" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="24" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A24" s="9" t="s">
+    <row r="24" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A24" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="B24" s="9" t="s">
+      <c r="B24" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="C24" s="15" t="s">
+      <c r="C24" s="9" t="s">
         <v>44</v>
       </c>
-      <c r="D24" s="15"/>
+      <c r="D24" s="9"/>
     </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A1:E1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
+  <pageSetup orientation="landscape" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -1421,201 +1862,195 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A2:A36"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A6" activeCellId="1" sqref="A4 A6 A8 A10 A13 A17 A21 A23 A29 A34"/>
-      <pivotSelection pane="bottomRight" showHeader="1" axis="axisRow" activeRow="5" previousRow="5" click="1" r:id="rId1">
-        <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
-          <references count="1">
-            <reference field="0" count="0"/>
-          </references>
-        </pivotArea>
-      </pivotSelection>
+    <sheetView tabSelected="1" topLeftCell="A23" workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="138.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="74.7109375" style="18" customWidth="1"/>
     <col min="2" max="2" width="16.28515625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="11.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A2" s="10" t="s">
+      <c r="A2" s="15" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
+      <c r="A3" s="16" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A4" s="2" t="s">
+      <c r="A4" s="17" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A5" s="3" t="s">
+    <row r="5" spans="1:1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A5" s="17" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A6" s="2" t="s">
+      <c r="A6" s="17" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A7" s="3" t="s">
+      <c r="A7" s="17" t="s">
         <v>52</v>
       </c>
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A8" s="2" t="s">
+      <c r="A8" s="17" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A9" s="3" t="s">
+      <c r="A9" s="17" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="10" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A10" s="2" t="s">
+      <c r="A10" s="17" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A11" s="3" t="s">
+    <row r="11" spans="1:1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A11" s="17" t="s">
         <v>53</v>
       </c>
     </row>
     <row r="12" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A12" s="3" t="s">
+      <c r="A12" s="17" t="s">
         <v>40</v>
       </c>
     </row>
     <row r="13" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A13" s="2" t="s">
+      <c r="A13" s="17" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="14" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A14" s="3" t="s">
+      <c r="A14" s="17" t="s">
         <v>54</v>
       </c>
     </row>
     <row r="15" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A15" s="3" t="s">
+      <c r="A15" s="17" t="s">
         <v>55</v>
       </c>
     </row>
     <row r="16" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A16" s="3" t="s">
+      <c r="A16" s="17" t="s">
         <v>56</v>
       </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A17" s="2" t="s">
+      <c r="A17" s="17" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A18" s="3" t="s">
+      <c r="A18" s="17" t="s">
         <v>57</v>
       </c>
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A19" s="3" t="s">
+      <c r="A19" s="17" t="s">
         <v>58</v>
       </c>
     </row>
     <row r="20" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A20" s="3" t="s">
+      <c r="A20" s="17" t="s">
         <v>59</v>
       </c>
     </row>
     <row r="21" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A21" s="2" t="s">
+      <c r="A21" s="17" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A22" s="3" t="s">
+    <row r="22" spans="1:1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A22" s="17" t="s">
         <v>60</v>
       </c>
     </row>
     <row r="23" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A23" s="2" t="s">
+      <c r="A23" s="17" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A24" s="3" t="s">
+    <row r="24" spans="1:1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A24" s="17" t="s">
         <v>61</v>
       </c>
     </row>
     <row r="25" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A25" s="3" t="s">
+      <c r="A25" s="17" t="s">
         <v>62</v>
       </c>
     </row>
     <row r="26" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A26" s="3" t="s">
+      <c r="A26" s="17" t="s">
         <v>63</v>
       </c>
     </row>
     <row r="27" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A27" s="3" t="s">
+      <c r="A27" s="17" t="s">
         <v>64</v>
       </c>
     </row>
     <row r="28" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A28" s="3" t="s">
+      <c r="A28" s="17" t="s">
         <v>65</v>
       </c>
     </row>
     <row r="29" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A29" s="2" t="s">
+      <c r="A29" s="17" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="30" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A30" s="3" t="s">
+      <c r="A30" s="17" t="s">
         <v>66</v>
       </c>
     </row>
     <row r="31" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A31" s="3" t="s">
+      <c r="A31" s="17" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="32" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A32" s="3" t="s">
+      <c r="A32" s="17" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A33" s="3" t="s">
+    <row r="33" spans="1:1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A33" s="17" t="s">
         <v>67</v>
       </c>
     </row>
     <row r="34" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A34" s="2" t="s">
+      <c r="A34" s="17" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="35" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A35" s="3" t="s">
+      <c r="A35" s="17" t="s">
         <v>68</v>
       </c>
     </row>
     <row r="36" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A36" s="2" t="s">
+      <c r="A36" s="17" t="s">
         <v>43</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -1827,10 +2262,16 @@
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A4D74005-AF0F-436E-A5ED-89FA61229623}">
   <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="d78dacd4-ba8a-4506-8839-a918012505f4"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="e62effa8-c612-4657-b64e-83124bbab7cb"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="e62effa8-c612-4657-b64e-83124bbab7cb"/>
-    <ds:schemaRef ds:uri="d78dacd4-ba8a-4506-8839-a918012505f4"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>